<commit_message>
recfactoritzat les funcions de mostra(:)
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M17"/>
+  <dimension ref="C2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="M13" sqref="M10:M13"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
@@ -619,6 +619,86 @@
       <c r="I17" s="7"/>
       <c r="J17" s="1"/>
     </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>